<commit_message>
kiwoom real sw 2nd day added
</commit_message>
<xml_diff>
--- a/태영 시간표_학원.xlsx
+++ b/태영 시간표_학원.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
   <si>
     <t>월</t>
   </si>
@@ -113,6 +113,26 @@
   </si>
   <si>
     <t>연세바이올린첼로, 호수공원 앞</t>
+  </si>
+  <si>
+    <t>방과후(2학기)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>웹툰</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>화(15:40~17:10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>생명과학</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>금(15:00~16:00) or 16:10~17:10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -203,7 +223,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -215,6 +235,9 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="표준" xfId="0" builtinId="0"/>
@@ -498,7 +521,7 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -512,6 +535,7 @@
     <col min="8" max="8" width="14.75" customWidth="1"/>
     <col min="9" max="9" width="14.625" hidden="1" customWidth="1"/>
     <col min="10" max="11" width="16.75" customWidth="1"/>
+    <col min="13" max="13" width="35.625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
@@ -683,6 +707,9 @@
       <c r="J7" s="3" t="s">
         <v>19</v>
       </c>
+      <c r="L7" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -699,6 +726,12 @@
       </c>
       <c r="H8" s="9"/>
       <c r="I8" s="8"/>
+      <c r="L8" t="s">
+        <v>30</v>
+      </c>
+      <c r="M8" t="s">
+        <v>31</v>
+      </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -710,6 +743,12 @@
       <c r="C9" s="9"/>
       <c r="I9" s="8" t="s">
         <v>12</v>
+      </c>
+      <c r="L9" t="s">
+        <v>32</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
kiwoom develop 3 day added
</commit_message>
<xml_diff>
--- a/태영 시간표_학원.xlsx
+++ b/태영 시간표_학원.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="41">
   <si>
     <t>월</t>
   </si>
@@ -132,6 +132,34 @@
   </si>
   <si>
     <t>금(15:00~16:00) or 16:10~17:10)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>13:00~14:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>14:00~15:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>15:00~16:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16:00~17:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>17:00~18:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>18:00~19:00</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19:00~20:00</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -521,12 +549,13 @@
   <dimension ref="A1:M10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K15" sqref="K15"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.625" hidden="1" customWidth="1"/>
+    <col min="1" max="1" width="10.875" customWidth="1"/>
+    <col min="2" max="2" width="15.375" hidden="1" customWidth="1"/>
     <col min="3" max="3" width="14.625" customWidth="1"/>
     <col min="4" max="4" width="14.5" customWidth="1"/>
     <col min="5" max="5" width="16.25" hidden="1" customWidth="1"/>
@@ -616,8 +645,8 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="1">
-        <v>0.54166666666666663</v>
+      <c r="A4" s="1" t="s">
+        <v>34</v>
       </c>
       <c r="E4" s="6" t="s">
         <v>6</v>
@@ -632,8 +661,8 @@
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="1">
-        <v>0.58333333333333337</v>
+      <c r="A5" s="1" t="s">
+        <v>35</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -663,8 +692,8 @@
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" s="1">
-        <v>0.625</v>
+      <c r="A6" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="B6" s="2"/>
       <c r="C6" s="3" t="s">
@@ -683,8 +712,8 @@
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="1">
-        <v>0.66666666666666663</v>
+      <c r="A7" s="1" t="s">
+        <v>37</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>11</v>
@@ -692,7 +721,9 @@
       <c r="C7" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="7"/>
+      <c r="D7" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="E7" s="5" t="s">
         <v>7</v>
       </c>
@@ -700,7 +731,9 @@
         <v>7</v>
       </c>
       <c r="G7" s="4"/>
-      <c r="H7" s="9"/>
+      <c r="H7" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I7" s="8" t="s">
         <v>11</v>
       </c>
@@ -712,19 +745,20 @@
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" s="1">
-        <v>0.70833333333333337</v>
+      <c r="A8" s="1" t="s">
+        <v>38</v>
       </c>
       <c r="B8" s="8"/>
       <c r="C8" s="2" t="s">
         <v>22</v>
       </c>
+      <c r="D8" s="8"/>
       <c r="E8" s="5"/>
       <c r="F8" s="5"/>
       <c r="G8" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H8" s="9"/>
+      <c r="H8" s="8"/>
       <c r="I8" s="8"/>
       <c r="L8" t="s">
         <v>30</v>
@@ -734,13 +768,19 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A9" s="1">
-        <v>0.75</v>
+      <c r="A9" s="1" t="s">
+        <v>39</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="C9" s="9"/>
+      <c r="D9" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="H9" s="8" t="s">
+        <v>12</v>
+      </c>
       <c r="I9" s="8" t="s">
         <v>12</v>
       </c>
@@ -752,8 +792,8 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A10" s="1">
-        <v>0.79166666666666663</v>
+      <c r="A10" s="1" t="s">
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>